<commit_message>
ph as input results
</commit_message>
<xml_diff>
--- a/Nuno-dataset/ph-as-input/test-solidos-00/content/results/metrics_1_7.xlsx
+++ b/Nuno-dataset/ph-as-input/test-solidos-00/content/results/metrics_1_7.xlsx
@@ -482,28 +482,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9607363272723993</v>
+        <v>0.9716593622110361</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8577851262147558</v>
+        <v>0.9848163966797699</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9567897875592353</v>
+        <v>0.9714960963015005</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9057603735274234</v>
+        <v>0.9765106555253509</v>
       </c>
       <c r="F2" t="n">
-        <v>4.735210620945968</v>
+        <v>3.417889355224486</v>
       </c>
       <c r="G2" t="n">
-        <v>21.37937216480316</v>
+        <v>0.7288246990781945</v>
       </c>
       <c r="H2" t="n">
-        <v>3.910437667191649</v>
+        <v>3.707779310339084</v>
       </c>
       <c r="I2" t="n">
-        <v>13.15869853100757</v>
+        <v>2.130688651051019</v>
       </c>
     </row>
     <row r="3">
@@ -513,28 +513,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9622774711379214</v>
+        <v>0.9754610717835247</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8603910761185656</v>
+        <v>0.98074487231038</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9554085973131623</v>
+        <v>0.969521961585375</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9068244742305609</v>
+        <v>0.9740378568764824</v>
       </c>
       <c r="F3" t="n">
-        <v>4.549348211918295</v>
+        <v>2.959402048897043</v>
       </c>
       <c r="G3" t="n">
-        <v>20.98761586425955</v>
+        <v>0.9242610168431958</v>
       </c>
       <c r="H3" t="n">
-        <v>4.03543261766095</v>
+        <v>3.964574166710198</v>
       </c>
       <c r="I3" t="n">
-        <v>13.01011792979631</v>
+        <v>2.354993080796383</v>
       </c>
     </row>
     <row r="4">
@@ -544,710 +544,710 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9635068113859198</v>
+        <v>0.978283291144702</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8625652211147752</v>
+        <v>0.9752237606972762</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9539957372464617</v>
+        <v>0.9671772568083953</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9076327847850229</v>
+        <v>0.9709088005393038</v>
       </c>
       <c r="F4" t="n">
-        <v>4.401089411997466</v>
+        <v>2.619041553677957</v>
       </c>
       <c r="G4" t="n">
-        <v>20.66077343366821</v>
+        <v>1.189278643102976</v>
       </c>
       <c r="H4" t="n">
-        <v>4.163293623456074</v>
+        <v>4.269572666315571</v>
       </c>
       <c r="I4" t="n">
-        <v>12.8972533599363</v>
+        <v>2.638825813264546</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_3</t>
+          <t>model_1_7_24</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9644855728087803</v>
+        <v>0.9800541257333281</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8643827027127644</v>
+        <v>0.864867734621651</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9525882440929107</v>
+        <v>0.9276005173036169</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9082394128925712</v>
+        <v>0.9132842392344228</v>
       </c>
       <c r="F5" t="n">
-        <v>4.283050492993241</v>
+        <v>2.405478375057995</v>
       </c>
       <c r="G5" t="n">
-        <v>20.3875487388675</v>
+        <v>6.486453220159458</v>
       </c>
       <c r="H5" t="n">
-        <v>4.290668934362157</v>
+        <v>9.417703163059464</v>
       </c>
       <c r="I5" t="n">
-        <v>12.81254975184224</v>
+        <v>7.865876696979679</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_4</t>
+          <t>model_1_7_23</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9652630989087954</v>
+        <v>0.9802592904222188</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8659048923323142</v>
+        <v>0.8669152639502347</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9512125312364342</v>
+        <v>0.9283044223530015</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9086874595987239</v>
+        <v>0.9143329132306084</v>
       </c>
       <c r="F6" t="n">
-        <v>4.189280613838104</v>
+        <v>2.380735452493956</v>
       </c>
       <c r="G6" t="n">
-        <v>20.15871572361696</v>
+        <v>6.388170229272141</v>
       </c>
       <c r="H6" t="n">
-        <v>4.415168192045272</v>
+        <v>9.326139403717651</v>
       </c>
       <c r="I6" t="n">
-        <v>12.74998889761611</v>
+        <v>7.770752808582694</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_5</t>
+          <t>model_1_7_3</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9658791808475538</v>
+        <v>0.9803368263828021</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8671826439225819</v>
+        <v>0.9687486985154555</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9498868292314252</v>
+        <v>0.9646014748244854</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9090114219281097</v>
+        <v>0.9673565322058085</v>
       </c>
       <c r="F7" t="n">
-        <v>4.114980948597398</v>
+        <v>2.371384592562785</v>
       </c>
       <c r="G7" t="n">
-        <v>19.96662943857932</v>
+        <v>1.500086634239727</v>
       </c>
       <c r="H7" t="n">
-        <v>4.535141567852333</v>
+        <v>4.604629620229839</v>
       </c>
       <c r="I7" t="n">
-        <v>12.70475397057584</v>
+        <v>2.961047569254156</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_6</t>
+          <t>model_1_7_22</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9663657207865833</v>
+        <v>0.9804806830852195</v>
       </c>
       <c r="C8" t="n">
-        <v>0.868256885524179</v>
+        <v>0.8691694926151172</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9486234700627706</v>
+        <v>0.9290799057768044</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9092384076882806</v>
+        <v>0.9154878775671746</v>
       </c>
       <c r="F8" t="n">
-        <v>4.056304087092593</v>
+        <v>2.354035431420698</v>
       </c>
       <c r="G8" t="n">
-        <v>19.80513711091928</v>
+        <v>6.279965510426024</v>
       </c>
       <c r="H8" t="n">
-        <v>4.649473041854489</v>
+        <v>9.225264750733231</v>
       </c>
       <c r="I8" t="n">
-        <v>12.67305990194761</v>
+        <v>7.665987458193869</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_7</t>
+          <t>model_1_7_21</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9667486626932926</v>
+        <v>0.9807185674861527</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8691625259780796</v>
+        <v>0.8716489282469794</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9474298530817979</v>
+        <v>0.929933499552772</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9093905555085071</v>
+        <v>0.9167585325368609</v>
       </c>
       <c r="F9" t="n">
-        <v>4.010121179129926</v>
+        <v>2.325346501842686</v>
       </c>
       <c r="G9" t="n">
-        <v>19.66899084297912</v>
+        <v>6.160950683038639</v>
       </c>
       <c r="H9" t="n">
-        <v>4.757492987578985</v>
+        <v>9.114229526384877</v>
       </c>
       <c r="I9" t="n">
-        <v>12.65181547034862</v>
+        <v>7.550727957179093</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_8</t>
+          <t>model_1_7_20</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9670486702744083</v>
+        <v>0.9809728988564196</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8699272429700202</v>
+        <v>0.8743721170008409</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9463099428527737</v>
+        <v>0.9308722444758812</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9094848548800585</v>
+        <v>0.9181549127754154</v>
       </c>
       <c r="F10" t="n">
-        <v>3.973940175525932</v>
+        <v>2.294674062866275</v>
       </c>
       <c r="G10" t="n">
-        <v>19.55402980735541</v>
+        <v>6.030235517329467</v>
       </c>
       <c r="H10" t="n">
-        <v>4.8588426199015</v>
+        <v>8.992117866157329</v>
       </c>
       <c r="I10" t="n">
-        <v>12.63864842959991</v>
+        <v>7.424064076454329</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_9</t>
+          <t>model_1_7_19</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.9672825858912618</v>
+        <v>0.9812431181478899</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8705746299828115</v>
+        <v>0.8773588081325215</v>
       </c>
       <c r="D11" t="n">
-        <v>0.94526551534963</v>
+        <v>0.9319028726043962</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9095353288707977</v>
+        <v>0.9196871468803179</v>
       </c>
       <c r="F11" t="n">
-        <v>3.945729882489559</v>
+        <v>2.2620855358624</v>
       </c>
       <c r="G11" t="n">
-        <v>19.45670716090687</v>
+        <v>5.88687203374936</v>
       </c>
       <c r="H11" t="n">
-        <v>4.953361216738832</v>
+        <v>8.858054065915027</v>
       </c>
       <c r="I11" t="n">
-        <v>12.63160073583609</v>
+        <v>7.285077063785983</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_10</t>
+          <t>model_1_7_18</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.9674637512091444</v>
+        <v>0.9815281707907549</v>
       </c>
       <c r="C12" t="n">
-        <v>0.8711238028330041</v>
+        <v>0.8806295013575519</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9442959601962639</v>
+        <v>0.933032945786778</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9095526287471772</v>
+        <v>0.9213661432553955</v>
       </c>
       <c r="F12" t="n">
-        <v>3.923881291214455</v>
+        <v>2.227708102263976</v>
       </c>
       <c r="G12" t="n">
-        <v>19.37414919467893</v>
+        <v>5.729876230102814</v>
       </c>
       <c r="H12" t="n">
-        <v>5.041104015905582</v>
+        <v>8.71105448266059</v>
       </c>
       <c r="I12" t="n">
-        <v>12.62918515052</v>
+        <v>7.132777431695592</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_11</t>
+          <t>model_1_7_4</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9676030610002956</v>
+        <v>0.9817902060680403</v>
       </c>
       <c r="C13" t="n">
-        <v>0.8715910848227034</v>
+        <v>0.9616992650088036</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9433994314964805</v>
+        <v>0.9619024732891264</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9095454885872534</v>
+        <v>0.9635602287494021</v>
       </c>
       <c r="F13" t="n">
-        <v>3.907080488924834</v>
+        <v>2.196106569807434</v>
       </c>
       <c r="G13" t="n">
-        <v>19.3039020025408</v>
+        <v>1.838464893062646</v>
       </c>
       <c r="H13" t="n">
-        <v>5.122238067309688</v>
+        <v>4.955714936726491</v>
       </c>
       <c r="I13" t="n">
-        <v>12.63018213252658</v>
+        <v>3.305405441788265</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_12</t>
+          <t>model_1_7_17</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.9677091794134184</v>
+        <v>0.9818261270113613</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8719893451858312</v>
+        <v>0.8842049774142495</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9425733164688007</v>
+        <v>0.934270186592942</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9095205603328509</v>
+        <v>0.9232026872530835</v>
       </c>
       <c r="F14" t="n">
-        <v>3.894282576707529</v>
+        <v>2.191774493348163</v>
       </c>
       <c r="G14" t="n">
-        <v>19.24403093353676</v>
+        <v>5.558250614883276</v>
       </c>
       <c r="H14" t="n">
-        <v>5.196999822441089</v>
+        <v>8.550114566797626</v>
       </c>
       <c r="I14" t="n">
-        <v>12.63366286984342</v>
+        <v>6.966186854540361</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_13</t>
+          <t>model_1_7_16</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9677890390735875</v>
+        <v>0.9821339803896</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8723296619356408</v>
+        <v>0.8881043373061259</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9418143798641974</v>
+        <v>0.9356216860246738</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9094830532637285</v>
+        <v>0.9252072389566453</v>
       </c>
       <c r="F15" t="n">
-        <v>3.884651477914474</v>
+        <v>2.154647284275202</v>
       </c>
       <c r="G15" t="n">
-        <v>19.19287061356149</v>
+        <v>5.371078325153612</v>
       </c>
       <c r="H15" t="n">
-        <v>5.265682064855883</v>
+        <v>8.3743119229242</v>
       </c>
       <c r="I15" t="n">
-        <v>12.6388999896606</v>
+        <v>6.784356511431659</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_14</t>
+          <t>model_1_7_15</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.9678482546783576</v>
+        <v>0.9824473786204768</v>
       </c>
       <c r="C16" t="n">
-        <v>0.8726213259988023</v>
+        <v>0.8923471621862017</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9411186380332481</v>
+        <v>0.9370951306360364</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9094370983995587</v>
+        <v>0.9273900803298957</v>
       </c>
       <c r="F16" t="n">
-        <v>3.877510058348905</v>
+        <v>2.116851364323202</v>
       </c>
       <c r="G16" t="n">
-        <v>19.14902432387701</v>
+        <v>5.167419450429012</v>
       </c>
       <c r="H16" t="n">
-        <v>5.328645306846754</v>
+        <v>8.182646686375257</v>
       </c>
       <c r="I16" t="n">
-        <v>12.64531667684706</v>
+        <v>6.586353738470117</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_15</t>
+          <t>model_1_7_14</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.9678913024249027</v>
+        <v>0.9827603018442608</v>
       </c>
       <c r="C17" t="n">
-        <v>0.8728719374923004</v>
+        <v>0.8969507144418781</v>
       </c>
       <c r="D17" t="n">
-        <v>0.9404823232647397</v>
+        <v>0.9386970811675567</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9093858698519153</v>
+        <v>0.9297608767426826</v>
       </c>
       <c r="F17" t="n">
-        <v>3.872318487298915</v>
+        <v>2.079112730368037</v>
       </c>
       <c r="G17" t="n">
-        <v>19.11134952766432</v>
+        <v>4.946445382767233</v>
       </c>
       <c r="H17" t="n">
-        <v>5.386230518731018</v>
+        <v>7.974265437975578</v>
       </c>
       <c r="I17" t="n">
-        <v>12.65246972954743</v>
+        <v>6.371301802213261</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_16</t>
+          <t>model_1_7_5</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.9679217431295908</v>
+        <v>0.9827780740769174</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8730877882374959</v>
+        <v>0.9543630733737788</v>
       </c>
       <c r="D18" t="n">
-        <v>0.9399016432844698</v>
+        <v>0.9591626388857829</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9093317764289492</v>
+        <v>0.9596560485181792</v>
       </c>
       <c r="F18" t="n">
-        <v>3.86864732925041</v>
+        <v>2.076969393818305</v>
       </c>
       <c r="G18" t="n">
-        <v>19.07890036611913</v>
+        <v>2.190607763764036</v>
       </c>
       <c r="H18" t="n">
-        <v>5.438780893727309</v>
+        <v>5.312111780538692</v>
       </c>
       <c r="I18" t="n">
-        <v>12.66002280538148</v>
+        <v>3.659548679770158</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_17</t>
+          <t>model_1_7_13</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.9679423204381352</v>
+        <v>0.9830644498226336</v>
       </c>
       <c r="C19" t="n">
-        <v>0.8732738755275617</v>
+        <v>0.9019292724863923</v>
       </c>
       <c r="D19" t="n">
-        <v>0.9393721579541187</v>
+        <v>0.9404340966277315</v>
       </c>
       <c r="E19" t="n">
-        <v>0.9092763615535925</v>
+        <v>0.9323279294874226</v>
       </c>
       <c r="F19" t="n">
-        <v>3.86616569971346</v>
+        <v>2.042432393622112</v>
       </c>
       <c r="G19" t="n">
-        <v>19.05092558877297</v>
+        <v>4.707470747293065</v>
       </c>
       <c r="H19" t="n">
-        <v>5.486698255459071</v>
+        <v>7.748314983851841</v>
       </c>
       <c r="I19" t="n">
-        <v>12.6677603958861</v>
+        <v>6.138447702952643</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_24</t>
+          <t>model_1_7_12</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.9679536156842322</v>
+        <v>0.9833485627855617</v>
       </c>
       <c r="C20" t="n">
-        <v>0.8740476489762962</v>
+        <v>0.907292644421922</v>
       </c>
       <c r="D20" t="n">
-        <v>0.936802857363221</v>
+        <v>0.942311009251482</v>
       </c>
       <c r="E20" t="n">
-        <v>0.9089337658766374</v>
+        <v>0.9350969318102217</v>
       </c>
       <c r="F20" t="n">
-        <v>3.86480348967122</v>
+        <v>2.008168285703856</v>
       </c>
       <c r="G20" t="n">
-        <v>18.93460308261431</v>
+        <v>4.450024747518507</v>
       </c>
       <c r="H20" t="n">
-        <v>5.719214812112368</v>
+        <v>7.504166748323563</v>
       </c>
       <c r="I20" t="n">
-        <v>12.71559710110042</v>
+        <v>5.887275013553438</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_18</t>
+          <t>model_1_7_6</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.9679554229360092</v>
+        <v>0.9834073627166362</v>
       </c>
       <c r="C21" t="n">
-        <v>0.8734351290420459</v>
+        <v>0.9469559630897382</v>
       </c>
       <c r="D21" t="n">
-        <v>0.9388903455783514</v>
+        <v>0.9564432814882547</v>
       </c>
       <c r="E21" t="n">
-        <v>0.9092213311053243</v>
+        <v>0.9557457098326577</v>
       </c>
       <c r="F21" t="n">
-        <v>3.864585534568843</v>
+        <v>2.001076996509724</v>
       </c>
       <c r="G21" t="n">
-        <v>19.02668410961344</v>
+        <v>2.546154784451291</v>
       </c>
       <c r="H21" t="n">
-        <v>5.530301310299464</v>
+        <v>5.665844981528398</v>
       </c>
       <c r="I21" t="n">
-        <v>12.67544430875685</v>
+        <v>4.014250543332102</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_23</t>
+          <t>model_1_7_11</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.9679589474513823</v>
+        <v>0.9835978729382344</v>
       </c>
       <c r="C22" t="n">
-        <v>0.8739765421611002</v>
+        <v>0.9130443212462059</v>
       </c>
       <c r="D22" t="n">
-        <v>0.9370709191202212</v>
+        <v>0.9443305197724386</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9089750141188847</v>
+        <v>0.9380712330437556</v>
       </c>
       <c r="F22" t="n">
-        <v>3.86416047696548</v>
+        <v>1.978101407064259</v>
       </c>
       <c r="G22" t="n">
-        <v>18.94529267523613</v>
+        <v>4.173939812852931</v>
       </c>
       <c r="H22" t="n">
-        <v>5.694955760085161</v>
+        <v>7.241469420763858</v>
       </c>
       <c r="I22" t="n">
-        <v>12.70983760050624</v>
+        <v>5.617479920295843</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_19</t>
+          <t>model_1_7_7</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.9679627986250463</v>
+        <v>0.9837631836973593</v>
       </c>
       <c r="C23" t="n">
-        <v>0.873575066282391</v>
+        <v>0.9396361975231755</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9384523688361304</v>
+        <v>0.9537897467301758</v>
       </c>
       <c r="E23" t="n">
-        <v>0.9091675232099747</v>
+        <v>0.951904418112702</v>
       </c>
       <c r="F23" t="n">
-        <v>3.863696024274998</v>
+        <v>1.95816488029573</v>
       </c>
       <c r="G23" t="n">
-        <v>19.00564713744996</v>
+        <v>2.897509191166134</v>
       </c>
       <c r="H23" t="n">
-        <v>5.569937328115452</v>
+        <v>6.011015993167353</v>
       </c>
       <c r="I23" t="n">
-        <v>12.68295751631077</v>
+        <v>4.36268924420428</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_22</t>
+          <t>model_1_7_10</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.9679630975746411</v>
+        <v>0.9837929881258707</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8738953346608279</v>
+        <v>0.9191798639985141</v>
       </c>
       <c r="D24" t="n">
-        <v>0.9373669648788594</v>
+        <v>0.9464936275046365</v>
       </c>
       <c r="E24" t="n">
-        <v>0.9090190080423503</v>
+        <v>0.9412497785252237</v>
       </c>
       <c r="F24" t="n">
-        <v>3.863659970864864</v>
+        <v>1.95457045734356</v>
       </c>
       <c r="G24" t="n">
-        <v>18.95750071877394</v>
+        <v>3.879429016843496</v>
       </c>
       <c r="H24" t="n">
-        <v>5.668164211967268</v>
+        <v>6.96009301070043</v>
       </c>
       <c r="I24" t="n">
-        <v>12.70369471987578</v>
+        <v>5.329158090305105</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_21</t>
+          <t>model_1_7_9</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.9679656450601239</v>
+        <v>0.9839087252070432</v>
       </c>
       <c r="C25" t="n">
-        <v>0.8738027749388153</v>
+        <v>0.9256817332688343</v>
       </c>
       <c r="D25" t="n">
-        <v>0.9376940026203003</v>
+        <v>0.9487971509177602</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9090659996374946</v>
+        <v>0.944625924085317</v>
       </c>
       <c r="F25" t="n">
-        <v>3.863352743357165</v>
+        <v>1.940612530895684</v>
       </c>
       <c r="G25" t="n">
-        <v>18.97141535858416</v>
+        <v>3.567334264731977</v>
       </c>
       <c r="H25" t="n">
-        <v>5.638567951488866</v>
+        <v>6.660451370649861</v>
       </c>
       <c r="I25" t="n">
-        <v>12.69713327372898</v>
+        <v>5.022912207753948</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>model_1_7_20</t>
+          <t>model_1_7_8</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.9679658340578001</v>
+        <v>0.98391263573567</v>
       </c>
       <c r="C26" t="n">
-        <v>0.8736966970808925</v>
+        <v>0.932518281531611</v>
       </c>
       <c r="D26" t="n">
-        <v>0.9380548575084573</v>
+        <v>0.9512338685528039</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9091155931636918</v>
+        <v>0.9481855131970014</v>
       </c>
       <c r="F26" t="n">
-        <v>3.863329950181145</v>
+        <v>1.940140919979011</v>
       </c>
       <c r="G26" t="n">
-        <v>18.98736219974511</v>
+        <v>3.239174662214366</v>
       </c>
       <c r="H26" t="n">
-        <v>5.605911306975178</v>
+        <v>6.343483865850553</v>
       </c>
       <c r="I26" t="n">
-        <v>12.69020851941122</v>
+        <v>4.700026393258097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>